<commit_message>
Added analyzer and data supplier
</commit_message>
<xml_diff>
--- a/src/main/java/com/utils/OrangeHRM.xlsx
+++ b/src/main/java/com/utils/OrangeHRM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\eclipse-workspace\OrangeHRM_PF\src\main\java\com\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57680A4D-B4C5-42E0-87EE-350F8EFB4DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41AEBBD-5DA7-4FB2-89D1-AF0C9A3D326D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{34921288-73AA-4B09-8814-24D7A913806C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{34921288-73AA-4B09-8814-24D7A913806C}"/>
   </bookViews>
   <sheets>
     <sheet name="admin_login" sheetId="1" r:id="rId1"/>
@@ -504,13 +504,13 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -518,7 +518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -537,21 +537,21 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -577,7 +577,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -620,17 +620,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -649,17 +649,17 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -679,7 +679,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -712,13 +712,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -726,7 +726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>

</xml_diff>